<commit_message>
Version last before release
</commit_message>
<xml_diff>
--- a/Exchange/OUT/Contractors.xlsx
+++ b/Exchange/OUT/Contractors.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Контрагент:</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Алкогольная фабрика</t>
+  </si>
+  <si>
+    <t>Пивоварня</t>
   </si>
 </sst>
 </file>
@@ -363,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -397,6 +400,11 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>